<commit_message>
Two new Bottleneck pptx and excel
</commit_message>
<xml_diff>
--- a/_Test/list bottlenecks.xlsx
+++ b/_Test/list bottlenecks.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28723"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9489EE3C-5D7E-413D-9968-861400670383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F57C7243-0486-475C-A9F9-77ABCA760F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>List of B-N</t>
   </si>
@@ -129,10 +129,31 @@
     <t>Function f_numPP line 673</t>
   </si>
   <si>
+    <t>17th March, 2025</t>
+  </si>
+  <si>
+    <t>23rd March, 2025</t>
+  </si>
+  <si>
+    <t>Removed the unnecessary numPP variable.</t>
+  </si>
+  <si>
+    <t>The function runtime has decreased by approximately 29%</t>
+  </si>
+  <si>
     <t>Function f_numP line 636</t>
   </si>
   <si>
-    <t>Function f_KK line line 534</t>
+    <t>20th March, 2025</t>
+  </si>
+  <si>
+    <t>25th March, 2025</t>
+  </si>
+  <si>
+    <t>Removed the unnecessary numP variable.</t>
+  </si>
+  <si>
+    <t>Function runtime has negligible runtime compared to program runtime(Almost 95% decrease).</t>
   </si>
   <si>
     <t>Function digam all lines 879-884</t>
@@ -520,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -664,30 +685,55 @@
       <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="29.25">
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.5">
       <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="29.25">
-      <c r="B11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="29.25">
-      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="29.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>